<commit_message>
Performs API calculations for empty seats per port
</commit_message>
<xml_diff>
--- a/Notes/Schedule.xlsx
+++ b/Notes/Schedule.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Date</t>
   </si>
@@ -37,6 +37,12 @@
   </si>
   <si>
     <t>Available</t>
+  </si>
+  <si>
+    <t>New Reservation</t>
+  </si>
+  <si>
+    <t>Accepted</t>
   </si>
 </sst>
 </file>
@@ -44,7 +50,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$]dd/mm/yyyy;@" x16r2:formatCode16="[$-en-VG,1]dd/mm/yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="[$]dd/mm/yyyy;@" x16r2:formatCode16="[$-en-VG,1]dd/mm/yyyy;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -75,19 +81,53 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -363,40 +403,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="H7:M10"/>
+  <dimension ref="H7:O10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="14.7109375" style="2" customWidth="1"/>
-    <col min="9" max="13" width="14.7109375" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" style="1" customWidth="1"/>
+    <col min="9" max="15" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="8:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="8:15" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="H7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="J7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="K7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="L7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="M7" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="N7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="8" spans="8:13" x14ac:dyDescent="0.25">
-      <c r="H8" s="2">
+    <row r="8" spans="8:15" x14ac:dyDescent="0.25">
+      <c r="H8" s="1">
         <v>44440</v>
       </c>
       <c r="I8">
@@ -406,17 +452,25 @@
         <v>2</v>
       </c>
       <c r="K8">
-        <v>185</v>
+        <v>100</v>
       </c>
       <c r="L8">
         <v>100</v>
       </c>
       <c r="M8">
-        <v>85</v>
+        <f>K8-L8</f>
+        <v>0</v>
+      </c>
+      <c r="N8" s="6">
+        <v>300</v>
+      </c>
+      <c r="O8" s="5" t="str">
+        <f>IF(M9-N8&gt;=0,"YES","NO")</f>
+        <v>NO</v>
       </c>
     </row>
-    <row r="9" spans="8:13" x14ac:dyDescent="0.25">
-      <c r="H9" s="2">
+    <row r="9" spans="8:15" x14ac:dyDescent="0.25">
+      <c r="H9" s="1">
         <v>44440</v>
       </c>
       <c r="I9">
@@ -426,28 +480,45 @@
         <v>3</v>
       </c>
       <c r="K9">
-        <f>400-K8</f>
-        <v>215</v>
+        <v>100</v>
       </c>
       <c r="L9">
         <v>85</v>
       </c>
       <c r="M9">
         <f>K10-M8</f>
-        <v>315</v>
-      </c>
+        <v>200</v>
+      </c>
+      <c r="N9" s="6"/>
+      <c r="O9" s="5"/>
     </row>
-    <row r="10" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="8:15" x14ac:dyDescent="0.25">
       <c r="K10">
         <f>SUM(K8:K9)</f>
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="L10">
         <f>SUM(L8:L9)</f>
         <v>185</v>
       </c>
+      <c r="M10">
+        <f>K10-L10</f>
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="N8:N9"/>
+  </mergeCells>
+  <conditionalFormatting sqref="O8:O9">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="YES">
+      <formula>NOT(ISERROR(SEARCH("YES",O8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="NO">
+      <formula>NOT(ISERROR(SEARCH("NO",O8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>